<commit_message>
Rename temperature accuracy to uncertainty
Column description is made more generate. Source files are renamed.
References to column in notes are updated.

Closes #67.
</commit_message>
<xml_diff>
--- a/submission/template.xlsx
+++ b/submission/template.xlsx
@@ -258,8 +258,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>[number: °C] temperature_accuracy
-Thermistor accuracy or precision (as reported). Typically understood to represent one standard deviation.</t>
+          <t>[number: °C] temperature_uncertainty
+Estimated temperature uncertainty (as reported).</t>
         </r>
       </text>
     </comment>
@@ -461,7 +461,7 @@
     <t>to_bed</t>
   </si>
   <si>
-    <t>temperature_accuracy</t>
+    <t>temperature_uncertainty</t>
   </si>
   <si>
     <t>notes</t>
@@ -876,7 +876,7 @@
     <col min="11" max="11" width="15.140625" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" customWidth="1"/>
     <col min="13" max="14" width="10.7109375" customWidth="1"/>
-    <col min="15" max="15" width="24.7109375" customWidth="1"/>
+    <col min="15" max="15" width="28.28515625" customWidth="1"/>
     <col min="16" max="16" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Move borehole-level funding to borehole.funding
</commit_message>
<xml_diff>
--- a/submission/template.xlsx
+++ b/submission/template.xlsx
@@ -279,6 +279,22 @@
         </r>
       </text>
     </comment>
+    <comment ref="Q1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[string] funding
+Funding sources as a pipe-delimited list. Each entry must be in the format {funder} [{rorid}] &gt; {award} [{number}] ({url}), where only the funder is required, funder and award cannot contain parentheses, and rorid is the funder's ROR (https://ror.org) ID (e.g. 01jtrvx49).
+constraints:
+  - pattern: [^\s]+( [^\s]+)*</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -417,7 +433,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>id</t>
   </si>
@@ -465,6 +481,9 @@
   </si>
   <si>
     <t>notes</t>
+  </si>
+  <si>
+    <t>funding</t>
   </si>
   <si>
     <t>borehole_id</t>
@@ -858,7 +877,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -877,10 +896,10 @@
     <col min="12" max="12" width="11.5703125" customWidth="1"/>
     <col min="13" max="14" width="10.7109375" customWidth="1"/>
     <col min="15" max="15" width="28.28515625" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" customWidth="1"/>
+    <col min="16" max="17" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -928,32 +947,35 @@
       </c>
       <c r="P1" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A1048576">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>OR(AND(ISBLANK(A2), COUNTBLANK($A2:$P2) &lt;&gt; 16), IF(ISBLANK(A2), FALSE, OR(IF(ISNUMBER(A2), INT(A2) &lt;&gt; A2, TRUE), COUNTIF(A$2:A$1048576, A2) &gt;= 2, A2 &lt; 1)))</formula>
+      <formula>OR(AND(ISBLANK(A2), COUNTBLANK($A2:$Q2) &lt;&gt; 17), IF(ISBLANK(A2), FALSE, OR(IF(ISNUMBER(A2), INT(A2) &lt;&gt; A2, TRUE), COUNTIF(A$2:A$1048576, A2) &gt;= 2, A2 &lt; 1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AND(ISBLANK(B2), COUNTBLANK($A2:$P2) &lt;&gt; 16)</formula>
+      <formula>AND(ISBLANK(B2), COUNTBLANK($A2:$Q2) &lt;&gt; 17)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D1048576">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>OR(AND(ISBLANK(D2), COUNTBLANK($A2:$P2) &lt;&gt; 16), IF(ISBLANK(D2), FALSE, OR(NOT(ISNUMBER(D2)), D2 &lt; -90, D2 &gt; 90)))</formula>
+      <formula>OR(AND(ISBLANK(D2), COUNTBLANK($A2:$Q2) &lt;&gt; 17), IF(ISBLANK(D2), FALSE, OR(NOT(ISNUMBER(D2)), D2 &lt; -90, D2 &gt; 90)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E1048576">
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>OR(AND(ISBLANK(E2), COUNTBLANK($A2:$P2) &lt;&gt; 16), IF(ISBLANK(E2), FALSE, OR(NOT(ISNUMBER(E2)), E2 &lt; -180, E2 &gt; 180)))</formula>
+      <formula>OR(AND(ISBLANK(E2), COUNTBLANK($A2:$Q2) &lt;&gt; 17), IF(ISBLANK(E2), FALSE, OR(NOT(ISNUMBER(E2)), E2 &lt; -180, E2 &gt; 180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048576">
     <cfRule type="expression" dxfId="0" priority="5">
-      <formula>OR(AND(ISBLANK(F2), COUNTBLANK($A2:$P2) &lt;&gt; 16), IF(ISBLANK(F2), FALSE, OR(NOT(ISNUMBER(F2)), F2 &gt; 9999.0)))</formula>
+      <formula>OR(AND(ISBLANK(F2), COUNTBLANK($A2:$Q2) &lt;&gt; 17), IF(ISBLANK(F2), FALSE, OR(NOT(ISNUMBER(F2)), F2 &gt; 9999.0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G1048576">
@@ -1023,13 +1045,13 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -1038,13 +1060,13 @@
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1101,26 +1123,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add investigators from gastaldello2024
* Add borehole.investigators column
</commit_message>
<xml_diff>
--- a/submission/template.xlsx
+++ b/submission/template.xlsx
@@ -288,8 +288,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>[string] investigators
+Names of people and/or agencies who performed the work, as a pipe-delimited list. Each entry should be in the format {person} ({agencies}) [{notes}], where either person or at least one (semicolon-delimited) agencies is required.
+constraints:
+  - pattern: [^\s]+( [^\s]+)*</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>[string] funding
-Funding sources as a pipe-delimited list. Each entry must be in the format {funder} [{rorid}] &gt; {award} [{number}] ({url}), where only the funder is required, funder and award cannot contain parentheses, and rorid is the funder's ROR (https://ror.org) ID (e.g. 01jtrvx49).
+Funding sources as a pipe-delimited list. Each entry should be in the format {funder} [{rorid}] &gt; {award} [{number}] ({url}), where only the funder is required and rorid is the funder's ROR (https://ror.org) ID (e.g. 01jtrvx49).
 constraints:
   - pattern: [^\s]+( [^\s]+)*</t>
         </r>
@@ -433,7 +449,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>id</t>
   </si>
@@ -481,6 +497,9 @@
   </si>
   <si>
     <t>notes</t>
+  </si>
+  <si>
+    <t>investigators</t>
   </si>
   <si>
     <t>funding</t>
@@ -877,7 +896,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -896,10 +915,12 @@
     <col min="12" max="12" width="11.5703125" customWidth="1"/>
     <col min="13" max="14" width="10.7109375" customWidth="1"/>
     <col min="15" max="15" width="28.28515625" customWidth="1"/>
-    <col min="16" max="17" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -950,32 +971,35 @@
       </c>
       <c r="Q1" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A1048576">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>OR(AND(ISBLANK(A2), COUNTBLANK($A2:$Q2) &lt;&gt; 17), IF(ISBLANK(A2), FALSE, OR(IF(ISNUMBER(A2), INT(A2) &lt;&gt; A2, TRUE), COUNTIF(A$2:A$1048576, A2) &gt;= 2, A2 &lt; 1)))</formula>
+      <formula>OR(AND(ISBLANK(A2), COUNTBLANK($A2:$R2) &lt;&gt; 18), IF(ISBLANK(A2), FALSE, OR(IF(ISNUMBER(A2), INT(A2) &lt;&gt; A2, TRUE), COUNTIF(A$2:A$1048576, A2) &gt;= 2, A2 &lt; 1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AND(ISBLANK(B2), COUNTBLANK($A2:$Q2) &lt;&gt; 17)</formula>
+      <formula>AND(ISBLANK(B2), COUNTBLANK($A2:$R2) &lt;&gt; 18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D1048576">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>OR(AND(ISBLANK(D2), COUNTBLANK($A2:$Q2) &lt;&gt; 17), IF(ISBLANK(D2), FALSE, OR(NOT(ISNUMBER(D2)), D2 &lt; -90, D2 &gt; 90)))</formula>
+      <formula>OR(AND(ISBLANK(D2), COUNTBLANK($A2:$R2) &lt;&gt; 18), IF(ISBLANK(D2), FALSE, OR(NOT(ISNUMBER(D2)), D2 &lt; -90, D2 &gt; 90)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E1048576">
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>OR(AND(ISBLANK(E2), COUNTBLANK($A2:$Q2) &lt;&gt; 17), IF(ISBLANK(E2), FALSE, OR(NOT(ISNUMBER(E2)), E2 &lt; -180, E2 &gt; 180)))</formula>
+      <formula>OR(AND(ISBLANK(E2), COUNTBLANK($A2:$R2) &lt;&gt; 18), IF(ISBLANK(E2), FALSE, OR(NOT(ISNUMBER(E2)), E2 &lt; -180, E2 &gt; 180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048576">
     <cfRule type="expression" dxfId="0" priority="5">
-      <formula>OR(AND(ISBLANK(F2), COUNTBLANK($A2:$Q2) &lt;&gt; 17), IF(ISBLANK(F2), FALSE, OR(NOT(ISNUMBER(F2)), F2 &gt; 9999.0)))</formula>
+      <formula>OR(AND(ISBLANK(F2), COUNTBLANK($A2:$R2) &lt;&gt; 18), IF(ISBLANK(F2), FALSE, OR(NOT(ISNUMBER(F2)), F2 &gt; 9999.0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G1048576">
@@ -1045,13 +1069,13 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -1060,13 +1084,13 @@
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1123,26 +1147,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add borehole columns funding and investigators (#82)
* Drop unecessary quoting in borehole.csv
* Move borehole-level funding to borehole.funding
* Update gastaldello2024 submission
* Add funding from gastaldello2024
* Allow awards without titles
* Add borehole.investigators column
* Add investigators from gastaldello2024
</commit_message>
<xml_diff>
--- a/submission/template.xlsx
+++ b/submission/template.xlsx
@@ -279,6 +279,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="Q1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[string] investigators
+Names of people and/or agencies who performed the work, as a pipe-delimited list. Each entry should be in the format {person} ({agencies}) [{notes}], where either person or at least one (semicolon-delimited) agencies is required.
+constraints:
+  - pattern: [^\s]+( [^\s]+)*</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[string] funding
+Funding sources as a pipe-delimited list. Each entry should be in the format {funder} [{rorid}] &gt; {award} [{number}] ({url}), where only the funder is required and rorid is the funder's ROR (https://ror.org) ID (e.g. 01jtrvx49).
+constraints:
+  - pattern: [^\s]+( [^\s]+)*</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -417,7 +449,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>id</t>
   </si>
@@ -465,6 +497,12 @@
   </si>
   <si>
     <t>notes</t>
+  </si>
+  <si>
+    <t>investigators</t>
+  </si>
+  <si>
+    <t>funding</t>
   </si>
   <si>
     <t>borehole_id</t>
@@ -858,7 +896,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -878,9 +916,11 @@
     <col min="13" max="14" width="10.7109375" customWidth="1"/>
     <col min="15" max="15" width="28.28515625" customWidth="1"/>
     <col min="16" max="16" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -928,32 +968,38 @@
       </c>
       <c r="P1" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A1048576">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>OR(AND(ISBLANK(A2), COUNTBLANK($A2:$P2) &lt;&gt; 16), IF(ISBLANK(A2), FALSE, OR(IF(ISNUMBER(A2), INT(A2) &lt;&gt; A2, TRUE), COUNTIF(A$2:A$1048576, A2) &gt;= 2, A2 &lt; 1)))</formula>
+      <formula>OR(AND(ISBLANK(A2), COUNTBLANK($A2:$R2) &lt;&gt; 18), IF(ISBLANK(A2), FALSE, OR(IF(ISNUMBER(A2), INT(A2) &lt;&gt; A2, TRUE), COUNTIF(A$2:A$1048576, A2) &gt;= 2, A2 &lt; 1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AND(ISBLANK(B2), COUNTBLANK($A2:$P2) &lt;&gt; 16)</formula>
+      <formula>AND(ISBLANK(B2), COUNTBLANK($A2:$R2) &lt;&gt; 18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D1048576">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>OR(AND(ISBLANK(D2), COUNTBLANK($A2:$P2) &lt;&gt; 16), IF(ISBLANK(D2), FALSE, OR(NOT(ISNUMBER(D2)), D2 &lt; -90, D2 &gt; 90)))</formula>
+      <formula>OR(AND(ISBLANK(D2), COUNTBLANK($A2:$R2) &lt;&gt; 18), IF(ISBLANK(D2), FALSE, OR(NOT(ISNUMBER(D2)), D2 &lt; -90, D2 &gt; 90)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E1048576">
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>OR(AND(ISBLANK(E2), COUNTBLANK($A2:$P2) &lt;&gt; 16), IF(ISBLANK(E2), FALSE, OR(NOT(ISNUMBER(E2)), E2 &lt; -180, E2 &gt; 180)))</formula>
+      <formula>OR(AND(ISBLANK(E2), COUNTBLANK($A2:$R2) &lt;&gt; 18), IF(ISBLANK(E2), FALSE, OR(NOT(ISNUMBER(E2)), E2 &lt; -180, E2 &gt; 180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048576">
     <cfRule type="expression" dxfId="0" priority="5">
-      <formula>OR(AND(ISBLANK(F2), COUNTBLANK($A2:$P2) &lt;&gt; 16), IF(ISBLANK(F2), FALSE, OR(NOT(ISNUMBER(F2)), F2 &gt; 9999.0)))</formula>
+      <formula>OR(AND(ISBLANK(F2), COUNTBLANK($A2:$R2) &lt;&gt; 18), IF(ISBLANK(F2), FALSE, OR(NOT(ISNUMBER(F2)), F2 &gt; 9999.0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G1048576">
@@ -1023,13 +1069,13 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -1038,13 +1084,13 @@
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1101,26 +1147,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Chinese boreholes listed in Huang 1982
borehole.investigators format updated to support latinized form in square brackets
</commit_message>
<xml_diff>
--- a/submission/template.xlsx
+++ b/submission/template.xlsx
@@ -289,7 +289,7 @@
             <family val="2"/>
           </rPr>
           <t>[string] investigators
-Names of people and/or agencies who performed the work, as a pipe-delimited list. Each entry should be in the format {person} ({agencies}) [{notes}], where either person or at least one (semicolon-delimited) agencies is required.
+Names of people and/or agencies who performed the work, as a pipe-delimited list. Each entry should be in the format 'person (agency; ...) {notes}', where only person or one agency is required. Person and agency may contain a latinized form in square brackets.
 constraints:
   - pattern: [^\s]+( [^\s]+)*</t>
         </r>
@@ -305,7 +305,7 @@
             <family val="2"/>
           </rPr>
           <t>[string] funding
-Funding sources as a pipe-delimited list. Each entry should be in the format {funder} [{rorid}] &gt; {award} [{number}] ({url}), where only the funder is required and rorid is the funder's ROR (https://ror.org) ID (e.g. 01jtrvx49).
+Funding sources as a pipe-delimited list. Each entry should be in the format 'funder [rorid] &gt; award [number] (url)', where only funder is required and rorid is the funder's ROR (https://ror.org) ID (e.g. 01jtrvx49).
 constraints:
   - pattern: [^\s]+( [^\s]+)*</t>
         </r>

</xml_diff>

<commit_message>
Allow parentheses in funder and award names
</commit_message>
<xml_diff>
--- a/submission/template.xlsx
+++ b/submission/template.xlsx
@@ -289,7 +289,7 @@
             <family val="2"/>
           </rPr>
           <t>[string] investigators
-Names of people and/or agencies who performed the work, as a pipe-delimited list. Each entry should be in the format 'person (agency; ...) {notes}', where only person or one agency is required. Person and agency may contain a latinized form in square brackets.
+Names of people and/or agencies who performed the work, as a pipe-delimited list. Each entry is in the format 'person (agency; ...) {notes}', where only person or one agency is required. Person and agency may contain a latinized form in square brackets.
 constraints:
   - pattern: [^\s]+( [^\s]+)*</t>
         </r>
@@ -305,7 +305,7 @@
             <family val="2"/>
           </rPr>
           <t>[string] funding
-Funding sources as a pipe-delimited list. Each entry should be in the format 'funder [rorid] &gt; award [number] (url)', where only funder is required and rorid is the funder's ROR (https://ror.org) ID (e.g. 01jtrvx49).
+Funding sources as a pipe-delimited list. Each entry is in the format 'funder [rorid] &gt; award [number] url', where only funder is required and rorid is the funder's ROR (https://ror.org) ID (e.g. 01jtrvx49).
 constraints:
   - pattern: [^\s]+( [^\s]+)*</t>
         </r>

</xml_diff>

<commit_message>
Backfill profile.equilibrated column (and more)
* Backfill profile.equilibrated column (see #65)
* Replace boolean borehole.equilibrated with categorical
  borehole.equilibrium: true, estimated, false (see #96)
* Update other data in the process
</commit_message>
<xml_diff>
--- a/submission/template.xlsx
+++ b/submission/template.xlsx
@@ -439,8 +439,13 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>[boolean] equilibrated
-Whether temperatures have equilibrated following drilling.</t>
+          <t>[string] equilibrium
+Whether and how reported temperatures equilibrated following drilling.
+- true: Equilibrium was measured
+- estimated: Equilibrium was estimated (typically by extrapolation)
+- false: Equilibrium was not reached
+constraints:
+  - enum: ['true', 'estimated', 'false']</t>
         </r>
       </text>
     </comment>
@@ -449,7 +454,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>id</t>
   </si>
@@ -517,15 +522,12 @@
     <t>utc_offset</t>
   </si>
   <si>
-    <t>equilibrated</t>
+    <t>equilibrium</t>
   </si>
   <si>
     <t>ablation</t>
   </si>
   <si>
-    <t>equilibrium</t>
-  </si>
-  <si>
     <t>accumulation</t>
   </si>
   <si>
@@ -536,6 +538,15 @@
   </si>
   <si>
     <t>combined</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>estimated</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1075,7 @@
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="6" width="10.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1121,7 +1132,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H1048576">
     <cfRule type="expression" dxfId="0" priority="6">
-      <formula>IF(ISBLANK(H2), FALSE, AND(H2 &lt;&gt; TRUE, H2 &lt;&gt; FALSE))</formula>
+      <formula>IF(ISBLANK(H2), FALSE, ISNA(MATCH(H2, 'lists'!$C$1:$C$3, 0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -1129,7 +1140,7 @@
       <formula1>'borehole'!$A$2:$A$1048576</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in the dropdown list" sqref="H2:H1048576">
-      <formula1>"TRUE,FALSE"</formula1>
+      <formula1>'lists'!$C$1:$C$3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1139,34 +1150,43 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
+      <c r="C3" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>